<commit_message>
Marking Very Old Date and Handling Invalid Date
- Parsed date is compared with 2000-01-01 and is marked as True in the IsDateOld Column.
-  No dropping or segregating of this record is done.
-Invalid date is set to its next valid date,
eg 2022-02-30 is set to 2022-03-01. 2022-04-31 is set to 2022-05-01.
</commit_message>
<xml_diff>
--- a/InvalidRecords/InValidRows.xlsx
+++ b/InvalidRecords/InValidRows.xlsx
@@ -1,29 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s97ra\OneDrive\Desktop\Concordia\winter24\IP\Project\SSIS-ETL-TASK\InvalidRecords\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" url="C:\Users\s97ra\OneDrive\Desktop\Concordia\winter24\IP\Project\SSIS-ETL-TASK\InvalidRecords\"/>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB4DB92-3FDD-4920-86CA-B503A9559A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="InValidUserID" sheetId="2" r:id="rId2"/>
-    <sheet name="InValidAge" sheetId="3" r:id="rId3"/>
-    <sheet name="InValidEmail" sheetId="4" r:id="rId4"/>
+    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
+    <sheet sheetId="2" r:id="rId2" name="InValidUserID"/>
+    <sheet sheetId="3" r:id="rId3" name="InValidAge"/>
+    <sheet sheetId="4" r:id="rId4" name="InValidEmail"/>
   </sheets>
   <definedNames>
-    <definedName name="InValidAge">InValidAge!$A$1:$G$5</definedName>
-    <definedName name="InValidEmail">InValidEmail!$A$1:$G$2</definedName>
-    <definedName name="InValidUserID">InValidUserID!$A$1:$G$2</definedName>
+    <definedName name="InValidAge">'InValidAge'!$A$1:$G$5</definedName>
+    <definedName name="InValidEmail">'InValidEmail'!$A$1:$G$2</definedName>
+    <definedName name="InValidUserID">'InValidUserID'!$A$1:$G$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -487,51 +483,75 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
+    <row spans="1:7" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>UserID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>FullName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>RegistrationDate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>LastLoginDate</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>PurchaseTotal</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
+    <row spans="1:7" x14ac:dyDescent="0.3" outlineLevel="0" r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Null User</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2020-12-01</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2023-02-25</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -540,120 +560,191 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
+    <row spans="1:7" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>UserID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>FullName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>RegistrationDate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>LastLoginDate</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>PurchaseTotal</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
+    <row spans="1:7" x14ac:dyDescent="0.3" outlineLevel="0" r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Alice Johnson</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>alicejohnson@example.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2022-07-15</t>
+        </is>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
+    <row spans="1:7" x14ac:dyDescent="0.3" outlineLevel="0" r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Cathy Smith</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>cathysmith@example.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2019-10-12</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>210.5</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
+    <row spans="1:7" x14ac:dyDescent="0.3" outlineLevel="0" r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Eva Green</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>evagreen@example.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2018-08-22</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2023-02-23</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
+    <row spans="1:7" x14ac:dyDescent="0.3" outlineLevel="0" r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>121</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Kevin Yolt</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>kevinyolt@example.com</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2021-03-14</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2023-02-17</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -662,10 +753,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -676,50 +767,78 @@
     <col min="7" max="7" width="30.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
+    <row spans="1:7" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>UserID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>FullName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>RegistrationDate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>LastLoginDate</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>PurchaseTotal</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
+    <row spans="1:7" x14ac:dyDescent="0.3" outlineLevel="0" r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Incorrect Email</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>notanemail</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Date and Email checking script to handle emails with special characters.
</commit_message>
<xml_diff>
--- a/InvalidRecords/InValidRows.xlsx
+++ b/InvalidRecords/InValidRows.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="InValidAge">'InValidAge'!$A$1:$G$5</definedName>
-    <definedName name="InValidEmail">'InValidEmail'!$A$1:$G$2</definedName>
+    <definedName name="InValidEmail">'InValidEmail'!$A$1:$G$3</definedName>
     <definedName name="InValidUserID">'InValidUserID'!$A$1:$G$2</definedName>
   </definedNames>
   <calcPr calcId="162913" fullCalcOnLoad="true"/>
@@ -754,7 +754,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
@@ -807,35 +807,72 @@
     <row spans="1:7" x14ac:dyDescent="0.3" outlineLevel="0" r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>131</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Special Characters Name</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>special$$name@example.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2021-04-17</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2023-02-07</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>200.5</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
           <t>137</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>Incorrect Email</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>28</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>notanemail</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E3" s="0" t="inlineStr">
         <is>
           <t>2021-11-11</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F3" s="0" t="inlineStr">
         <is>
           <t>2023-02-01</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G3" s="0" t="inlineStr">
         <is>
           <t>190</t>
         </is>

</xml_diff>